<commit_message>
Made some tests and images for later use
</commit_message>
<xml_diff>
--- a/results/results_DryAllbestPartitions.xlsx
+++ b/results/results_DryAllbestPartitions.xlsx
@@ -423,577 +423,577 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1" t="n">
         <v>3</v>
       </c>
       <c r="G1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>3</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>3</v>
@@ -1002,60 +1002,60 @@
         <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -1067,57 +1067,57 @@
         <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>3</v>
@@ -1132,54 +1132,54 @@
         <v>3</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>3</v>
@@ -1194,19 +1194,19 @@
         <v>3</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O13" t="n">
         <v>2</v>
@@ -1215,33 +1215,33 @@
         <v>2</v>
       </c>
       <c r="Q13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>3</v>
@@ -1256,19 +1256,19 @@
         <v>3</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O14" t="n">
         <v>2</v>
@@ -1291,19 +1291,19 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>3</v>
@@ -1315,22 +1315,22 @@
         <v>3</v>
       </c>
       <c r="I15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O15" t="n">
         <v>2</v>
@@ -1353,19 +1353,19 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>3</v>
@@ -1374,25 +1374,25 @@
         <v>3</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O16" t="n">
         <v>2</v>
@@ -1415,46 +1415,46 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>3</v>
       </c>
       <c r="G17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O17" t="n">
         <v>2</v>
@@ -1477,46 +1477,46 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>3</v>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O18" t="n">
         <v>2</v>
@@ -1539,46 +1539,46 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>3</v>
       </c>
       <c r="G19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O19" t="n">
         <v>2</v>
@@ -1601,46 +1601,46 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
         <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O20" t="n">
         <v>2</v>
@@ -1663,46 +1663,46 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O21" t="n">
         <v>2</v>
@@ -1725,46 +1725,46 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O22" t="n">
         <v>2</v>
@@ -1787,46 +1787,46 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>3</v>
       </c>
       <c r="G23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O23" t="n">
         <v>2</v>
@@ -1849,46 +1849,46 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>3</v>
       </c>
       <c r="G24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O24" t="n">
         <v>2</v>
@@ -1911,46 +1911,46 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>3</v>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O25" t="n">
         <v>2</v>
@@ -1973,46 +1973,46 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
         <v>3</v>
       </c>
       <c r="G26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O26" t="n">
         <v>2</v>
@@ -2035,43 +2035,43 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N27" t="n">
         <v>2</v>
@@ -2097,43 +2097,43 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28" t="n">
         <v>2</v>
@@ -2159,43 +2159,43 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N29" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
more images and fixes
</commit_message>
<xml_diff>
--- a/results/results_DryAllbestPartitions.xlsx
+++ b/results/results_DryAllbestPartitions.xlsx
@@ -423,970 +423,970 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
         <v>3</v>
@@ -1395,60 +1395,60 @@
         <v>3</v>
       </c>
       <c r="O16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M17" t="n">
         <v>3</v>
@@ -1457,60 +1457,60 @@
         <v>3</v>
       </c>
       <c r="O17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M18" t="n">
         <v>3</v>
@@ -1519,704 +1519,704 @@
         <v>3</v>
       </c>
       <c r="O18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" t="n">
         <v>3</v>
       </c>
       <c r="O19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N20" t="n">
         <v>3</v>
       </c>
       <c r="O20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N21" t="n">
         <v>3</v>
       </c>
       <c r="O21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N22" t="n">
         <v>3</v>
       </c>
       <c r="O22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N23" t="n">
         <v>3</v>
       </c>
       <c r="O23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N24" t="n">
         <v>3</v>
       </c>
       <c r="O24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N25" t="n">
         <v>3</v>
       </c>
       <c r="O25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N26" t="n">
         <v>3</v>
       </c>
       <c r="O26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M27" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M28" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>